<commit_message>
Add monitor site IWIP
</commit_message>
<xml_diff>
--- a/data/iwip-sites.xlsx
+++ b/data/iwip-sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277E9AA7-2357-4439-9358-B564024380B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6F3E4D-DACB-4EE7-A644-6D1031E0C93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>ME-D7-WDA</t>
   </si>
   <si>
-    <t>L2SW</t>
-  </si>
-  <si>
     <t>SW-D7-NEWSSU020</t>
   </si>
   <si>
@@ -126,12 +123,6 @@
     <t>172.25.106.9</t>
   </si>
   <si>
-    <t>mf19980917</t>
-  </si>
-  <si>
-    <t>Dece2002</t>
-  </si>
-  <si>
     <t>xgigaethernet 1/0/39</t>
   </si>
   <si>
@@ -246,9 +237,6 @@
     <t>172.31.242.183</t>
   </si>
   <si>
-    <t>mso7-fikria</t>
-  </si>
-  <si>
     <t>GigabitEthernet2/1/0</t>
   </si>
   <si>
@@ -301,6 +289,18 @@
   </si>
   <si>
     <t>display interface GigabitEthernet2/1/3</t>
+  </si>
+  <si>
+    <t>L2SW FH S5800v3</t>
+  </si>
+  <si>
+    <t>L2SW FH S5800v2</t>
+  </si>
+  <si>
+    <t>username_nms</t>
+  </si>
+  <si>
+    <t>password_nms</t>
   </si>
 </sst>
 </file>
@@ -641,17 +641,17 @@
   <dimension ref="A1:AG54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -722,25 +722,25 @@
         <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -752,28 +752,28 @@
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -782,31 +782,31 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -815,31 +815,31 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -848,31 +848,31 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -881,31 +881,31 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -914,31 +914,31 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -947,31 +947,31 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="F9" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -980,31 +980,31 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="I10" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1013,31 +1013,31 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -1046,31 +1046,31 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -1079,31 +1079,31 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -1112,31 +1112,31 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -1145,31 +1145,31 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="I15" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -1178,31 +1178,31 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -1211,31 +1211,31 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -1244,31 +1244,31 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -1277,31 +1277,31 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="I19" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -1310,31 +1310,31 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -1343,31 +1343,31 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -1376,31 +1376,31 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -1409,31 +1409,31 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -1442,31 +1442,31 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="I24" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -1475,31 +1475,31 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -1508,31 +1508,31 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -1541,31 +1541,31 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>10</v>
@@ -1583,22 +1583,22 @@
         <v>4</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>10</v>
@@ -1616,22 +1616,22 @@
         <v>4</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E29" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="I29" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -1640,31 +1640,31 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -1673,31 +1673,31 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -1706,31 +1706,31 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -1739,31 +1739,31 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I33" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -1784,19 +1784,19 @@
         <v>11</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -1817,19 +1817,19 @@
         <v>11</v>
       </c>
       <c r="E35" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I35" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>

</xml_diff>